<commit_message>
database plan visual design done
</commit_message>
<xml_diff>
--- a/MCraftingTree.xlsx
+++ b/MCraftingTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danit\Desktop\MCraftingTree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DF6EE1-077B-452F-A9BD-306D263BBBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9C748B-71E4-498F-98E9-68B174516CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,12 +297,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -748,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -760,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -803,7 +811,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -811,18 +819,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -832,10 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -845,8 +855,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1187,8 +1198,8 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,7 +1268,7 @@
       <c r="D2" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="60" t="s">
         <v>83</v>
       </c>
       <c r="F2" s="46"/>
@@ -1498,7 +1509,7 @@
     </row>
     <row r="14" spans="1:21" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1525,52 +1536,52 @@
       <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="59"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
@@ -1582,14 +1593,14 @@
       <c r="A4" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="21"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
@@ -1601,14 +1612,14 @@
       <c r="A5" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="29"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -1620,15 +1631,15 @@
       <c r="A6" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -1639,14 +1650,14 @@
       <c r="A7" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="30"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
@@ -1658,14 +1669,14 @@
       <c r="A8" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
       <c r="H8" s="29"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
@@ -1677,15 +1688,15 @@
       <c r="A9" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -1696,14 +1707,14 @@
       <c r="A10" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
       <c r="H10" s="30"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
@@ -1715,14 +1726,14 @@
       <c r="A11" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="21"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
@@ -1734,14 +1745,14 @@
       <c r="A12" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="21"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
@@ -1753,14 +1764,14 @@
       <c r="A13" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
       <c r="H13" s="21"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
@@ -1772,14 +1783,14 @@
       <c r="A14" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="29"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
@@ -1791,15 +1802,15 @@
       <c r="A15" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
@@ -1810,15 +1821,15 @@
       <c r="A16" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -1829,14 +1840,14 @@
       <c r="A17" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
       <c r="H17" s="25"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -1848,15 +1859,15 @@
       <c r="A18" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
@@ -1867,14 +1878,14 @@
       <c r="A19" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="30"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -1886,14 +1897,14 @@
       <c r="A20" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="21"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
@@ -1905,14 +1916,14 @@
       <c r="A21" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
       <c r="H21" s="29"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
@@ -1924,15 +1935,15 @@
       <c r="A22" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
@@ -1943,14 +1954,14 @@
       <c r="A23" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
       <c r="H23" s="30"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
@@ -1962,14 +1973,14 @@
       <c r="A24" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
       <c r="H24" s="21"/>
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
@@ -1981,13 +1992,13 @@
       <c r="A25" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="30"/>
       <c r="H25" s="21"/>
       <c r="I25" s="19"/>
@@ -2000,13 +2011,13 @@
       <c r="A26" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="19"/>
@@ -2019,11 +2030,11 @@
       <c r="A27" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
       <c r="G27" s="22"/>
@@ -2037,16 +2048,12 @@
     <row r="28" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B2:M2"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B18:H18"/>
@@ -2058,12 +2065,16 @@
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B25:F25"/>
     <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B1:M1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>